<commit_message>
Running the notebooks to review data based on report findings
</commit_message>
<xml_diff>
--- a/Python Working Notebooks/Production Tank Model results in Excel format/26MT excel results/26 Agitation results/26results - AG Overall.xlsx
+++ b/Python Working Notebooks/Production Tank Model results in Excel format/26MT excel results/26 Agitation results/26results - AG Overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Thesis 2023\Capstone---CCT\Python Working Notebooks\Production Tank Model results in Excel format\26MT excel results\26 Agitation results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474E98E2-341F-4CE2-8F52-5C807C5F2566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397ED91D-B7AC-4395-B7C9-83A742FF6E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -403,6 +403,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,7 +1336,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="11" max="11" width="26.28515625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1385,28 +1397,28 @@
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="33">
         <v>3.2483399293662993E-2</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="34">
         <v>9.4142485098027862E-2</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="33">
         <v>0.31771473488846602</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="34">
         <v>0.45156274261001478</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="33">
         <v>0.96825907840447789</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="34">
         <v>0.90800934313278414</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="33">
         <v>0.2756104044542973</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="34">
         <v>-2.9563053150833959E-2</v>
       </c>
       <c r="K3" s="23" t="s">
@@ -1431,8 +1443,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="27" customWidth="1"/>
+    <col min="1" max="1" width="14" style="27" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="27" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="27"/>
     <col min="4" max="4" width="10" style="27" customWidth="1"/>
     <col min="5" max="10" width="9.140625" style="27"/>
@@ -1490,11 +1502,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="25.5">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:11" ht="38.25">
+      <c r="A3" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="25">

</xml_diff>